<commit_message>
update for hardware construction
</commit_message>
<xml_diff>
--- a/ETC module pin usage.xlsx
+++ b/ETC module pin usage.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="860" yWindow="1620" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="32720" windowHeight="20560" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PINS" sheetId="1" r:id="rId1"/>
     <sheet name="BOM" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="ETC_mod_bom" localSheetId="1">BOM!$A$1:$F$113</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId4"/>
+    <pivotCache cacheId="4" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="330">
   <si>
     <t>APPSA</t>
   </si>
@@ -1025,6 +1027,15 @@
   </si>
   <si>
     <t>Count of Part</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>6 WEEKS TO PAY</t>
+  </si>
+  <si>
+    <t>100 per week</t>
   </si>
 </sst>
 </file>
@@ -1092,13 +1103,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2160,7 +2178,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:C52" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField dataField="1" compact="0" outline="0" showAll="0">
@@ -2554,6 +2572,634 @@
   <dataFields count="1">
     <dataField name="Count of Part" fld="0" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:F152" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="105">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="52"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="55"/>
+        <item x="56"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="59"/>
+        <item x="60"/>
+        <item x="61"/>
+        <item x="44"/>
+        <item x="62"/>
+        <item x="63"/>
+        <item x="64"/>
+        <item x="65"/>
+        <item x="66"/>
+        <item x="67"/>
+        <item x="68"/>
+        <item x="69"/>
+        <item x="70"/>
+        <item x="71"/>
+        <item x="45"/>
+        <item x="72"/>
+        <item x="73"/>
+        <item x="74"/>
+        <item x="75"/>
+        <item x="76"/>
+        <item x="77"/>
+        <item x="78"/>
+        <item x="79"/>
+        <item x="80"/>
+        <item x="81"/>
+        <item x="46"/>
+        <item x="47"/>
+        <item x="48"/>
+        <item x="49"/>
+        <item x="50"/>
+        <item x="51"/>
+        <item x="82"/>
+        <item x="83"/>
+        <item x="84"/>
+        <item x="85"/>
+        <item x="92"/>
+        <item x="93"/>
+        <item x="94"/>
+        <item x="95"/>
+        <item x="96"/>
+        <item x="97"/>
+        <item x="98"/>
+        <item x="99"/>
+        <item x="100"/>
+        <item x="101"/>
+        <item x="86"/>
+        <item x="87"/>
+        <item x="88"/>
+        <item x="89"/>
+        <item x="90"/>
+        <item x="91"/>
+        <item x="102"/>
+        <item x="103"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="44">
+        <item x="28"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="19"/>
+        <item x="27"/>
+        <item x="4"/>
+        <item x="2"/>
+        <item x="20"/>
+        <item x="3"/>
+        <item x="22"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="29"/>
+        <item x="24"/>
+        <item x="23"/>
+        <item x="21"/>
+        <item x="30"/>
+        <item x="7"/>
+        <item x="32"/>
+        <item x="31"/>
+        <item x="9"/>
+        <item x="33"/>
+        <item x="40"/>
+        <item x="1"/>
+        <item x="10"/>
+        <item x="39"/>
+        <item x="15"/>
+        <item x="11"/>
+        <item x="36"/>
+        <item x="34"/>
+        <item x="18"/>
+        <item x="37"/>
+        <item x="41"/>
+        <item x="13"/>
+        <item x="17"/>
+        <item x="38"/>
+        <item x="14"/>
+        <item x="16"/>
+        <item x="35"/>
+        <item x="12"/>
+        <item x="42"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="148">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="58"/>
+    </i>
+    <i r="1">
+      <x v="71"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="59"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="42"/>
+    </i>
+    <i r="1">
+      <x v="43"/>
+    </i>
+    <i r="1">
+      <x v="47"/>
+    </i>
+    <i r="1">
+      <x v="51"/>
+    </i>
+    <i r="1">
+      <x v="77"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="44"/>
+    </i>
+    <i r="1">
+      <x v="48"/>
+    </i>
+    <i r="1">
+      <x v="52"/>
+    </i>
+    <i r="1">
+      <x v="53"/>
+    </i>
+    <i r="1">
+      <x v="78"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="46"/>
+    </i>
+    <i r="1">
+      <x v="50"/>
+    </i>
+    <i r="1">
+      <x v="55"/>
+    </i>
+    <i r="1">
+      <x v="75"/>
+    </i>
+    <i r="1">
+      <x v="76"/>
+    </i>
+    <i r="1">
+      <x v="80"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="62"/>
+    </i>
+    <i r="1">
+      <x v="63"/>
+    </i>
+    <i r="1">
+      <x v="66"/>
+    </i>
+    <i r="1">
+      <x v="67"/>
+    </i>
+    <i r="1">
+      <x v="68"/>
+    </i>
+    <i r="1">
+      <x v="70"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x v="45"/>
+    </i>
+    <i r="1">
+      <x v="49"/>
+    </i>
+    <i r="1">
+      <x v="54"/>
+    </i>
+    <i r="1">
+      <x v="64"/>
+    </i>
+    <i r="1">
+      <x v="79"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x v="65"/>
+    </i>
+    <i r="1">
+      <x v="69"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x v="73"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x v="72"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x v="74"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x v="90"/>
+    </i>
+    <i r="1">
+      <x v="91"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x v="99"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i r="1">
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i r="1">
+      <x v="84"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i r="1">
+      <x v="81"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i r="1">
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i r="1">
+      <x v="86"/>
+    </i>
+    <i r="1">
+      <x v="88"/>
+    </i>
+    <i r="1">
+      <x v="95"/>
+    </i>
+    <i r="1">
+      <x v="97"/>
+    </i>
+    <i r="1">
+      <x v="100"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i r="1">
+      <x v="92"/>
+    </i>
+    <i r="1">
+      <x v="93"/>
+    </i>
+    <i r="1">
+      <x v="94"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i r="1">
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i r="1">
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x v="85"/>
+    </i>
+    <i r="1">
+      <x v="87"/>
+    </i>
+    <i r="1">
+      <x v="89"/>
+    </i>
+    <i r="1">
+      <x v="96"/>
+    </i>
+    <i r="1">
+      <x v="98"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i r="1">
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i r="1">
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i r="1">
+      <x v="82"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i r="1">
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i r="1">
+      <x v="101"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="29"/>
+    </i>
+    <i r="1">
+      <x v="39"/>
+    </i>
+    <i r="1">
+      <x v="83"/>
+    </i>
+    <i r="1">
+      <x v="102"/>
+    </i>
+    <i r="1">
+      <x v="103"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
   <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -3141,7 +3787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -5266,8 +5912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5813,4 +6459,829 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:A152"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A48" activeCellId="9" sqref="A6 A8:A9 A11 A13:A17 A19 A21:A23 A25:A37 A39:A43 A45:A46 A48:A53 A55 A57:A61 A63:A64 A66:A71 A73 A75 A77:A81 A83:A84 A86 A88 A90 A92 A94 A96:A97 A99 A101 A103 A105 A107 A109 A111 A113 A115:A119 A121:A123 A125 A127 A129:A133 A135 A137 A139 A141 A143 A145:A151"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:1">
+      <c r="A4" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="7" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="7" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="6">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="7" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="6">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="7" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="6">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="7" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="7" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="6" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="7" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="7" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="7" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="6" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="7" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="7" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="7" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="7" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="7" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="7" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="6" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="7" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="6" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="7" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="6" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="7" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="6" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="7" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="6" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="7" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="6" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="7" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="6" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="6" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="7" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="6" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="7" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="7" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="6" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="7" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="7" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="7" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="6" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="7" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="7" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="7" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="6" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="6" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C6:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="6" spans="3:4">
+      <c r="C6" s="8">
+        <v>42387</v>
+      </c>
+      <c r="D6" s="8">
+        <f>C6-10*7</f>
+        <v>42317</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4">
+      <c r="C7" s="8">
+        <f ca="1">TODAY()</f>
+        <v>42269</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4">
+      <c r="D10">
+        <f ca="1">D6-C7</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4">
+      <c r="D16">
+        <f ca="1">D10/7</f>
+        <v>6.8571428571428568</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" t="s">
+        <v>329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update to fix reverse polarity protection
FLIP DS  on FET, only done on ETC schematic
</commit_message>
<xml_diff>
--- a/ETC module pin usage.xlsx
+++ b/ETC module pin usage.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14000" yWindow="460" windowWidth="14000" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="PINS" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,11 @@
   </sheets>
   <definedNames>
     <definedName name="ETC_mod_bom" localSheetId="2">BOM!$A$1:$F$113</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">PINS!$A$1:$D$25</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1132,7 +1133,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1152,6 +1153,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1177,12 +1184,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1193,10 +1215,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1207,6 +1227,9 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2273,7 +2296,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" compact="0" compactData="0" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:C52" firstHeaderRow="2" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="6">
     <pivotField dataField="1" compact="0" outline="0" showAll="0">
@@ -2677,7 +2700,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="A3:F152" firstHeaderRow="2" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
@@ -3630,10 +3653,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3642,338 +3668,351 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>352</v>
       </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="7">
         <v>0</v>
       </c>
-      <c r="B2" t="str">
+      <c r="B2" s="7" t="str">
         <f>VLOOKUP(A2,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTB16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B3" s="7" t="str">
         <f>VLOOKUP(A3,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTB17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="7">
         <v>2</v>
       </c>
-      <c r="B4" t="str">
+      <c r="B4" s="7" t="str">
         <f>VLOOKUP(A4,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTD0</v>
       </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="7">
         <v>3</v>
       </c>
-      <c r="B5" t="str">
+      <c r="B5" s="7" t="str">
         <f>VLOOKUP(A5,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTA12</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="7">
         <v>4</v>
       </c>
-      <c r="B6" t="str">
+      <c r="B6" s="7" t="str">
         <f>VLOOKUP(A6,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTA13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="7">
         <v>5</v>
       </c>
-      <c r="B7" t="str">
+      <c r="B7" s="7" t="str">
         <f>VLOOKUP(A7,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTD7</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="7">
         <v>6</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B8" s="7" t="str">
         <f>VLOOKUP(A8,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTD4</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="7">
         <v>7</v>
       </c>
-      <c r="B9" t="str">
+      <c r="B9" s="7" t="str">
         <f>VLOOKUP(A9,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTD2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="7">
         <v>8</v>
       </c>
-      <c r="B10" t="str">
+      <c r="B10" s="7" t="str">
         <f>VLOOKUP(A10,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTD3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>354</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="7">
         <v>9</v>
       </c>
-      <c r="B11" t="str">
+      <c r="B11" s="7" t="str">
         <f>VLOOKUP(A11,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTC3</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="7">
         <v>10</v>
       </c>
-      <c r="B12" t="str">
+      <c r="B12" s="7" t="str">
         <f>VLOOKUP(A12,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTC4</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="7"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="7">
         <v>11</v>
       </c>
-      <c r="B13" t="str">
+      <c r="B13" s="7" t="str">
         <f>VLOOKUP(A13,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTC6</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="7">
         <v>12</v>
       </c>
-      <c r="B14" t="str">
+      <c r="B14" s="7" t="str">
         <f>VLOOKUP(A14,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTC7</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="7">
         <v>13</v>
       </c>
-      <c r="B15" t="str">
+      <c r="B15" s="7" t="str">
         <f>VLOOKUP(A15,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTC5</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
+      <c r="A16" s="9">
         <v>14</v>
       </c>
-      <c r="B16" t="str">
+      <c r="B16" s="7" t="str">
         <f>VLOOKUP(A16,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTD1</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="A17" s="9">
         <v>15</v>
       </c>
-      <c r="B17" t="str">
+      <c r="B17" s="7" t="str">
         <f>VLOOKUP(A17,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTC0</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
+      <c r="A18" s="9">
         <v>16</v>
       </c>
-      <c r="B18" t="str">
+      <c r="B18" s="7" t="str">
         <f>VLOOKUP(A18,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTB0</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
+      <c r="A19" s="9">
         <v>17</v>
       </c>
-      <c r="B19" t="str">
+      <c r="B19" s="7" t="str">
         <f>VLOOKUP(A19,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTB1</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="A20" s="9">
         <v>18</v>
       </c>
-      <c r="B20" t="str">
+      <c r="B20" s="7" t="str">
         <f>VLOOKUP(A20,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTB3</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="A21" s="9">
         <v>19</v>
       </c>
-      <c r="B21" t="str">
+      <c r="B21" s="7" t="str">
         <f>VLOOKUP(A21,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTB2</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="A22" s="9">
         <v>20</v>
       </c>
-      <c r="B22" t="str">
+      <c r="B22" s="7" t="str">
         <f>VLOOKUP(A22,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTD5</v>
       </c>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="A23" s="9">
         <v>21</v>
       </c>
-      <c r="B23" t="str">
+      <c r="B23" s="7" t="str">
         <f>VLOOKUP(A23,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTD6</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="A24" s="9">
         <v>22</v>
       </c>
-      <c r="B24" t="str">
+      <c r="B24" s="7" t="str">
         <f>VLOOKUP(A24,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTC1</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="A25" s="9">
         <v>23</v>
       </c>
-      <c r="B25" t="str">
+      <c r="B25" s="7" t="str">
         <f>VLOOKUP(A25,pin_mapping!$A$2:$B$25,2,0)</f>
         <v>PTC2</v>
       </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
 </file>
 
@@ -4211,12 +4250,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
@@ -4227,7 +4266,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B5" t="s">
@@ -4238,7 +4277,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
@@ -4246,7 +4285,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B9" t="s">
@@ -4266,7 +4305,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C11" t="s">
@@ -4283,7 +4322,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B12" t="s">
@@ -4303,7 +4342,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="1" t="s">
         <v>43</v>
       </c>
       <c r="C13" t="s">
@@ -4320,7 +4359,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B14" t="s">
@@ -4340,7 +4379,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B15" t="s">
@@ -4360,7 +4399,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B16" t="s">
@@ -4380,7 +4419,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B17" t="s">
@@ -4400,7 +4439,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B18" t="s">
@@ -4420,7 +4459,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B19" t="s">
@@ -4440,7 +4479,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="1" t="s">
         <v>67</v>
       </c>
       <c r="B20" t="s">
@@ -4460,7 +4499,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="1" t="s">
         <v>71</v>
       </c>
       <c r="B21" t="s">
@@ -4480,7 +4519,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B22" t="s">
@@ -4500,7 +4539,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="1" t="s">
         <v>75</v>
       </c>
       <c r="B23" t="s">
@@ -4520,7 +4559,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="1" t="s">
         <v>78</v>
       </c>
       <c r="B24" t="s">
@@ -4540,7 +4579,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
       <c r="B25" t="s">
@@ -4560,7 +4599,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B26" t="s">
@@ -4580,7 +4619,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B27" t="s">
@@ -4600,7 +4639,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B28" t="s">
@@ -4620,7 +4659,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B29" t="s">
@@ -4640,7 +4679,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B30" t="s">
@@ -4660,7 +4699,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B31" t="s">
@@ -4680,7 +4719,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B32" t="s">
@@ -4700,7 +4739,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B33" t="s">
@@ -4720,7 +4759,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B34" t="s">
@@ -4740,7 +4779,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B35" t="s">
@@ -4760,7 +4799,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B36" t="s">
@@ -4780,7 +4819,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B37" t="s">
@@ -4800,7 +4839,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B38" t="s">
@@ -4820,7 +4859,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B39" t="s">
@@ -4840,7 +4879,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C40" t="s">
@@ -4857,7 +4896,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B41" t="s">
@@ -4877,7 +4916,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B42" t="s">
@@ -4897,7 +4936,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B43" t="s">
@@ -4917,7 +4956,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="1" t="s">
         <v>130</v>
       </c>
       <c r="B44" t="s">
@@ -4937,7 +4976,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="1" t="s">
         <v>134</v>
       </c>
       <c r="B45" t="s">
@@ -4957,7 +4996,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="1" t="s">
         <v>139</v>
       </c>
       <c r="B46" t="s">
@@ -4977,7 +5016,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="1" t="s">
         <v>144</v>
       </c>
       <c r="B47" t="s">
@@ -4997,7 +5036,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="1" t="s">
         <v>148</v>
       </c>
       <c r="B48" t="s">
@@ -5017,7 +5056,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="1" t="s">
         <v>153</v>
       </c>
       <c r="B49" t="s">
@@ -5037,7 +5076,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="1" t="s">
         <v>157</v>
       </c>
       <c r="C50" t="s">
@@ -5054,7 +5093,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="1" t="s">
         <v>159</v>
       </c>
       <c r="B51" t="s">
@@ -5074,7 +5113,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="1" t="s">
         <v>161</v>
       </c>
       <c r="B52" t="s">
@@ -5094,7 +5133,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="1" t="s">
         <v>166</v>
       </c>
       <c r="B53">
@@ -5114,7 +5153,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="1" t="s">
         <v>169</v>
       </c>
       <c r="B54" t="s">
@@ -5134,7 +5173,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="1" t="s">
         <v>172</v>
       </c>
       <c r="B55" t="s">
@@ -5154,7 +5193,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="1" t="s">
         <v>175</v>
       </c>
       <c r="B56" t="s">
@@ -5174,7 +5213,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="1" t="s">
         <v>178</v>
       </c>
       <c r="B57" t="s">
@@ -5194,7 +5233,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="1" t="s">
         <v>180</v>
       </c>
       <c r="B58">
@@ -5214,7 +5253,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B59" t="s">
@@ -5234,7 +5273,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="3" t="s">
+      <c r="A60" s="1" t="s">
         <v>184</v>
       </c>
       <c r="B60" t="s">
@@ -5254,7 +5293,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
+      <c r="A61" s="1" t="s">
         <v>186</v>
       </c>
       <c r="B61" t="s">
@@ -5274,7 +5313,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="1" t="s">
         <v>188</v>
       </c>
       <c r="B62">
@@ -5294,7 +5333,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="1" t="s">
         <v>190</v>
       </c>
       <c r="B63" t="s">
@@ -5314,7 +5353,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="1" t="s">
         <v>192</v>
       </c>
       <c r="B64" t="s">
@@ -5334,7 +5373,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="1" t="s">
         <v>194</v>
       </c>
       <c r="B65" t="s">
@@ -5354,7 +5393,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="3" t="s">
+      <c r="A66" s="1" t="s">
         <v>196</v>
       </c>
       <c r="B66">
@@ -5374,7 +5413,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="1" t="s">
         <v>198</v>
       </c>
       <c r="B67" t="s">
@@ -5394,7 +5433,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="3" t="s">
+      <c r="A68" s="1" t="s">
         <v>200</v>
       </c>
       <c r="B68" t="s">
@@ -5414,7 +5453,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="3" t="s">
+      <c r="A69" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B69" t="s">
@@ -5434,7 +5473,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="1" t="s">
         <v>204</v>
       </c>
       <c r="B70">
@@ -5454,7 +5493,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="1" t="s">
         <v>206</v>
       </c>
       <c r="B71" t="s">
@@ -5474,7 +5513,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="3" t="s">
+      <c r="A72" s="1" t="s">
         <v>208</v>
       </c>
       <c r="B72" t="s">
@@ -5494,7 +5533,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="1" t="s">
         <v>210</v>
       </c>
       <c r="B73" t="s">
@@ -5514,7 +5553,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="1" t="s">
         <v>212</v>
       </c>
       <c r="B74" t="s">
@@ -5534,7 +5573,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="3" t="s">
+      <c r="A75" s="1" t="s">
         <v>216</v>
       </c>
       <c r="B75" t="s">
@@ -5554,7 +5593,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="1" t="s">
         <v>219</v>
       </c>
       <c r="B76">
@@ -5574,7 +5613,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="3" t="s">
+      <c r="A77" s="1" t="s">
         <v>221</v>
       </c>
       <c r="B77">
@@ -5594,7 +5633,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="1" t="s">
         <v>223</v>
       </c>
       <c r="B78">
@@ -5614,7 +5653,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="1" t="s">
         <v>225</v>
       </c>
       <c r="B79">
@@ -5634,7 +5673,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="3" t="s">
+      <c r="A80" s="1" t="s">
         <v>227</v>
       </c>
       <c r="B80" t="s">
@@ -5654,7 +5693,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="1" t="s">
         <v>230</v>
       </c>
       <c r="B81" t="s">
@@ -5674,7 +5713,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="3" t="s">
+      <c r="A82" s="1" t="s">
         <v>232</v>
       </c>
       <c r="B82" t="s">
@@ -5694,7 +5733,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="3" t="s">
+      <c r="A83" s="1" t="s">
         <v>235</v>
       </c>
       <c r="B83" t="s">
@@ -5714,7 +5753,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
+      <c r="A84" s="1" t="s">
         <v>237</v>
       </c>
       <c r="B84" t="s">
@@ -5734,7 +5773,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="1" t="s">
         <v>239</v>
       </c>
       <c r="B85" t="s">
@@ -5754,7 +5793,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="3" t="s">
+      <c r="A86" s="1" t="s">
         <v>241</v>
       </c>
       <c r="B86" t="s">
@@ -5774,7 +5813,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="3" t="s">
+      <c r="A87" s="1" t="s">
         <v>243</v>
       </c>
       <c r="B87" t="s">
@@ -5794,7 +5833,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
+      <c r="A88" s="1" t="s">
         <v>245</v>
       </c>
       <c r="B88">
@@ -5814,7 +5853,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="3" t="s">
+      <c r="A89" s="1" t="s">
         <v>247</v>
       </c>
       <c r="B89" t="s">
@@ -5834,7 +5873,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="1" t="s">
         <v>250</v>
       </c>
       <c r="B90" t="s">
@@ -5854,7 +5893,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="1" t="s">
         <v>253</v>
       </c>
       <c r="B91" t="s">
@@ -5874,7 +5913,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="3" t="s">
+      <c r="A92" s="1" t="s">
         <v>256</v>
       </c>
       <c r="B92" t="s">
@@ -5894,7 +5933,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
+      <c r="A93" s="1" t="s">
         <v>259</v>
       </c>
       <c r="B93" t="s">
@@ -5914,7 +5953,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="3" t="s">
+      <c r="A94" s="1" t="s">
         <v>263</v>
       </c>
       <c r="C94" t="s">
@@ -5931,7 +5970,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="1" t="s">
         <v>266</v>
       </c>
       <c r="B95" t="s">
@@ -5951,7 +5990,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="3" t="s">
+      <c r="A96" s="1" t="s">
         <v>270</v>
       </c>
       <c r="B96" t="s">
@@ -5971,7 +6010,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="3" t="s">
+      <c r="A97" s="1" t="s">
         <v>274</v>
       </c>
       <c r="B97" t="s">
@@ -5991,7 +6030,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="1" t="s">
         <v>277</v>
       </c>
       <c r="B98" t="s">
@@ -6011,7 +6050,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="3" t="s">
+      <c r="A99" s="1" t="s">
         <v>279</v>
       </c>
       <c r="B99" t="s">
@@ -6031,7 +6070,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="1" t="s">
         <v>281</v>
       </c>
       <c r="B100" t="s">
@@ -6051,7 +6090,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="3" t="s">
+      <c r="A101" s="1" t="s">
         <v>284</v>
       </c>
       <c r="B101" t="s">
@@ -6071,7 +6110,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="1" t="s">
         <v>286</v>
       </c>
       <c r="B102" t="s">
@@ -6091,7 +6130,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="3" t="s">
+      <c r="A103" s="1" t="s">
         <v>288</v>
       </c>
       <c r="B103" t="s">
@@ -6111,7 +6150,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="3" t="s">
+      <c r="A104" s="1" t="s">
         <v>290</v>
       </c>
       <c r="B104" t="s">
@@ -6131,7 +6170,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="1" t="s">
         <v>292</v>
       </c>
       <c r="B105" t="s">
@@ -6151,7 +6190,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="1" t="s">
         <v>294</v>
       </c>
       <c r="B106" t="s">
@@ -6171,7 +6210,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="3" t="s">
+      <c r="A107" s="1" t="s">
         <v>296</v>
       </c>
       <c r="B107" t="s">
@@ -6191,7 +6230,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="3" t="s">
+      <c r="A108" s="1" t="s">
         <v>300</v>
       </c>
       <c r="B108" t="s">
@@ -6211,7 +6250,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="3" t="s">
+      <c r="A109" s="1" t="s">
         <v>302</v>
       </c>
       <c r="B109" t="s">
@@ -6231,7 +6270,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" s="3" t="s">
+      <c r="A110" s="1" t="s">
         <v>306</v>
       </c>
       <c r="B110" t="s">
@@ -6251,7 +6290,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
+      <c r="A111" s="1" t="s">
         <v>308</v>
       </c>
       <c r="B111" t="s">
@@ -6271,7 +6310,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" s="3" t="s">
+      <c r="A112" s="1" t="s">
         <v>310</v>
       </c>
       <c r="B112" t="s">
@@ -6291,7 +6330,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" s="3" t="s">
+      <c r="A113" s="1" t="s">
         <v>315</v>
       </c>
       <c r="C113" t="s">
@@ -6329,15 +6368,15 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C4" t="s">
@@ -6351,7 +6390,7 @@
       <c r="B5" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6362,7 +6401,7 @@
       <c r="B6" t="s">
         <v>167</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>2</v>
       </c>
     </row>
@@ -6373,7 +6412,7 @@
       <c r="B7" t="s">
         <v>167</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6384,7 +6423,7 @@
       <c r="B8" t="s">
         <v>167</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>5</v>
       </c>
     </row>
@@ -6395,7 +6434,7 @@
       <c r="B9" t="s">
         <v>167</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6406,7 +6445,7 @@
       <c r="B10" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>3</v>
       </c>
     </row>
@@ -6417,7 +6456,7 @@
       <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>13</v>
       </c>
     </row>
@@ -6428,7 +6467,7 @@
       <c r="B12" t="s">
         <v>167</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>5</v>
       </c>
     </row>
@@ -6439,7 +6478,7 @@
       <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>2</v>
       </c>
     </row>
@@ -6450,7 +6489,7 @@
       <c r="B14" t="s">
         <v>167</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>6</v>
       </c>
     </row>
@@ -6461,7 +6500,7 @@
       <c r="B15" t="s">
         <v>119</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6472,7 +6511,7 @@
       <c r="B16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="3">
         <v>5</v>
       </c>
     </row>
@@ -6483,7 +6522,7 @@
       <c r="B17" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="3">
         <v>2</v>
       </c>
     </row>
@@ -6494,7 +6533,7 @@
       <c r="B18" t="s">
         <v>167</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="3">
         <v>6</v>
       </c>
     </row>
@@ -6505,7 +6544,7 @@
       <c r="B19" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6516,7 +6555,7 @@
       <c r="B20" t="s">
         <v>214</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6527,7 +6566,7 @@
       <c r="B21" t="s">
         <v>167</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="3">
         <v>5</v>
       </c>
     </row>
@@ -6538,7 +6577,7 @@
       <c r="B22" t="s">
         <v>167</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="3">
         <v>2</v>
       </c>
     </row>
@@ -6549,7 +6588,7 @@
       <c r="B23" t="s">
         <v>111</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6560,7 +6599,7 @@
       <c r="B24" t="s">
         <v>167</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6571,7 +6610,7 @@
       <c r="B25" t="s">
         <v>167</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6582,7 +6621,7 @@
       <c r="B26" t="s">
         <v>123</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6593,7 +6632,7 @@
       <c r="B27" t="s">
         <v>167</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6604,7 +6643,7 @@
       <c r="B28" t="s">
         <v>298</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="3">
         <v>2</v>
       </c>
     </row>
@@ -6615,7 +6654,7 @@
       <c r="B29" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6626,7 +6665,7 @@
       <c r="B30" t="s">
         <v>127</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6637,7 +6676,7 @@
       <c r="B31" t="s">
         <v>282</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6648,7 +6687,7 @@
       <c r="B32" t="s">
         <v>150</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6659,7 +6698,7 @@
       <c r="B33" t="s">
         <v>132</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6670,7 +6709,7 @@
       <c r="B34" t="s">
         <v>268</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6681,7 +6720,7 @@
       <c r="B35" t="s">
         <v>127</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6692,7 +6731,7 @@
       <c r="B36" t="s">
         <v>163</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6703,7 +6742,7 @@
       <c r="B37" t="s">
         <v>272</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="3">
         <v>5</v>
       </c>
     </row>
@@ -6714,7 +6753,7 @@
       <c r="B38" t="s">
         <v>304</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="3">
         <v>3</v>
       </c>
     </row>
@@ -6725,7 +6764,7 @@
       <c r="B39" t="s">
         <v>141</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6736,7 +6775,7 @@
       <c r="B40" t="s">
         <v>141</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6747,7 +6786,7 @@
       <c r="B41" t="s">
         <v>272</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="3">
         <v>5</v>
       </c>
     </row>
@@ -6758,7 +6797,7 @@
       <c r="B42" t="s">
         <v>146</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6769,7 +6808,7 @@
       <c r="B43" t="s">
         <v>155</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6780,7 +6819,7 @@
       <c r="B44" t="s">
         <v>261</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6791,7 +6830,7 @@
       <c r="B45" t="s">
         <v>136</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6802,7 +6841,7 @@
       <c r="B46" t="s">
         <v>312</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6813,7 +6852,7 @@
       <c r="B47" t="s">
         <v>33</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6821,7 +6860,7 @@
       <c r="B48" t="s">
         <v>316</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6829,7 +6868,7 @@
       <c r="B49" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="5">
+      <c r="C49" s="3">
         <v>3</v>
       </c>
     </row>
@@ -6837,7 +6876,7 @@
       <c r="B50" t="s">
         <v>264</v>
       </c>
-      <c r="C50" s="5">
+      <c r="C50" s="3">
         <v>1</v>
       </c>
     </row>
@@ -6845,13 +6884,13 @@
       <c r="B51" t="s">
         <v>318</v>
       </c>
-      <c r="C51" s="5"/>
+      <c r="C51" s="3"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>319</v>
       </c>
-      <c r="C52" s="5">
+      <c r="C52" s="3">
         <v>103</v>
       </c>
     </row>
@@ -6874,747 +6913,747 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6">
+      <c r="A5" s="4">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
+      <c r="A7" s="4">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
+      <c r="A10" s="4">
         <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6">
+      <c r="A12" s="4">
         <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="6">
+      <c r="A18" s="4">
         <v>680</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="5" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="5" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="5" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="5" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="5" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="5" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="5" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="4" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
+      <c r="A39" s="5" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="7" t="s">
+      <c r="A40" s="5" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="5" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="5" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="7" t="s">
+      <c r="A43" s="5" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="4" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="5" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="7" t="s">
+      <c r="A46" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="4" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="7" t="s">
+      <c r="A48" s="5" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="5" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="5" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="7" t="s">
+      <c r="A51" s="5" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="5" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="7" t="s">
+      <c r="A53" s="5" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="4" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="7" t="s">
+      <c r="A55" s="5" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="4" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="7" t="s">
+      <c r="A58" s="5" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="5" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="7" t="s">
+      <c r="A60" s="5" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="7" t="s">
+      <c r="A61" s="5" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="6" t="s">
+      <c r="A62" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="7" t="s">
+      <c r="A63" s="5" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="7" t="s">
+      <c r="A64" s="5" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="6" t="s">
+      <c r="A65" s="4" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="5" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="5" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="5" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="7" t="s">
+      <c r="A69" s="5" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="5" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="5" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="6" t="s">
+      <c r="A72" s="4" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="5" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="6" t="s">
+      <c r="A74" s="4" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="5" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="6" t="s">
+      <c r="A76" s="4" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="5" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="5" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="5" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="5" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="5" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="6" t="s">
+      <c r="A82" s="4" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="5" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="7" t="s">
+      <c r="A84" s="5" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="6" t="s">
+      <c r="A85" s="4" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="7" t="s">
+      <c r="A86" s="5" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="6" t="s">
+      <c r="A87" s="4" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="5" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A89" s="6" t="s">
+      <c r="A89" s="4" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="5" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A91" s="6" t="s">
+      <c r="A91" s="4" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="5" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A93" s="6" t="s">
+      <c r="A93" s="4" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A94" s="7" t="s">
+      <c r="A94" s="5" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A95" s="6" t="s">
+      <c r="A95" s="4" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A96" s="7" t="s">
+      <c r="A96" s="5" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="7" t="s">
+      <c r="A97" s="5" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A98" s="6" t="s">
+      <c r="A98" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A99" s="7" t="s">
+      <c r="A99" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A100" s="6" t="s">
+      <c r="A100" s="4" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="7" t="s">
+      <c r="A101" s="5" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A102" s="6" t="s">
+      <c r="A102" s="4" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A103" s="7" t="s">
+      <c r="A103" s="5" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A104" s="6" t="s">
+      <c r="A104" s="4" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="7" t="s">
+      <c r="A105" s="5" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="6" t="s">
+      <c r="A106" s="4" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="7" t="s">
+      <c r="A107" s="5" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A108" s="6" t="s">
+      <c r="A108" s="4" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109" s="7" t="s">
+      <c r="A109" s="5" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110" s="6" t="s">
+      <c r="A110" s="4" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111" s="7" t="s">
+      <c r="A111" s="5" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A112" s="6" t="s">
+      <c r="A112" s="4" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="7" t="s">
+      <c r="A113" s="5" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="6" t="s">
+      <c r="A114" s="4" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" s="7" t="s">
+      <c r="A115" s="5" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" s="7" t="s">
+      <c r="A116" s="5" t="s">
         <v>292</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A117" s="7" t="s">
+      <c r="A117" s="5" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A118" s="7" t="s">
+      <c r="A118" s="5" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" s="7" t="s">
+      <c r="A119" s="5" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120" s="6" t="s">
+      <c r="A120" s="4" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A121" s="7" t="s">
+      <c r="A121" s="5" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122" s="7" t="s">
+      <c r="A122" s="5" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123" s="7" t="s">
+      <c r="A123" s="5" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124" s="6" t="s">
+      <c r="A124" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A125" s="7" t="s">
+      <c r="A125" s="5" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A126" s="6" t="s">
+      <c r="A126" s="4" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127" s="7" t="s">
+      <c r="A127" s="5" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A128" s="6" t="s">
+      <c r="A128" s="4" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A129" s="7" t="s">
+      <c r="A129" s="5" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A130" s="7" t="s">
+      <c r="A130" s="5" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A131" s="7" t="s">
+      <c r="A131" s="5" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A132" s="7" t="s">
+      <c r="A132" s="5" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A133" s="7" t="s">
+      <c r="A133" s="5" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A134" s="6" t="s">
+      <c r="A134" s="4" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A135" s="7" t="s">
+      <c r="A135" s="5" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" s="6" t="s">
+      <c r="A136" s="4" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A137" s="7" t="s">
+      <c r="A137" s="5" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A138" s="6" t="s">
+      <c r="A138" s="4" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A139" s="7" t="s">
+      <c r="A139" s="5" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A140" s="6" t="s">
+      <c r="A140" s="4" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A141" s="7" t="s">
+      <c r="A141" s="5" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A142" s="6" t="s">
+      <c r="A142" s="4" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A143" s="7" t="s">
+      <c r="A143" s="5" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A144" s="6" t="s">
+      <c r="A144" s="4" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A145" s="7" t="s">
+      <c r="A145" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A146" s="7" t="s">
+      <c r="A146" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A147" s="7" t="s">
+      <c r="A147" s="5" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A148" s="7" t="s">
+      <c r="A148" s="5" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A149" s="7" t="s">
+      <c r="A149" s="5" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A150" s="7" t="s">
+      <c r="A150" s="5" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A151" s="7" t="s">
+      <c r="A151" s="5" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A152" s="6" t="s">
+      <c r="A152" s="4" t="s">
         <v>319</v>
       </c>
     </row>
@@ -7634,30 +7673,30 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="6" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>42387</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <f>C6-10*7</f>
         <v>42317</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <f ca="1">TODAY()</f>
-        <v>42316</v>
+        <v>42330</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D10">
         <f ca="1">D6-C7</f>
-        <v>1</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D16">
         <f ca="1">D10/7</f>
-        <v>0.14285714285714285</v>
+        <v>-1.8571428571428572</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updates with wiring updates
Woop
</commit_message>
<xml_diff>
--- a/ETC module pin usage.xlsx
+++ b/ETC module pin usage.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27860" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="14020" yWindow="460" windowWidth="14020" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="PINS" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="359">
   <si>
     <t>APPSA</t>
   </si>
@@ -1127,6 +1127,9 @@
   </si>
   <si>
     <t>I2C_DAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -3656,10 +3659,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3667,7 +3670,7 @@
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>351</v>
       </c>
@@ -3677,7 +3680,7 @@
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>0</v>
       </c>
@@ -3692,7 +3695,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -3707,7 +3710,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -3718,7 +3721,7 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -3733,7 +3736,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>4</v>
       </c>
@@ -3748,7 +3751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>5</v>
       </c>
@@ -3763,7 +3766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>6</v>
       </c>
@@ -3778,7 +3781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>7</v>
       </c>
@@ -3793,7 +3796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>8</v>
       </c>
@@ -3808,7 +3811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>9</v>
       </c>
@@ -3823,7 +3826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="7">
         <v>10</v>
       </c>
@@ -3834,7 +3837,7 @@
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>11</v>
       </c>
@@ -3845,7 +3848,7 @@
       <c r="C13" s="8"/>
       <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7">
         <v>12</v>
       </c>
@@ -3856,7 +3859,7 @@
       <c r="C14" s="8"/>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>13</v>
       </c>
@@ -3867,7 +3870,7 @@
       <c r="C15" s="8"/>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>14</v>
       </c>
@@ -3880,6 +3883,9 @@
       </c>
       <c r="D16" s="7" t="s">
         <v>13</v>
+      </c>
+      <c r="K16" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -7684,19 +7690,19 @@
     <row r="7" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C7" s="6">
         <f ca="1">TODAY()</f>
-        <v>42330</v>
+        <v>42337</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D10">
         <f ca="1">D6-C7</f>
-        <v>-13</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.2">
       <c r="D16">
         <f ca="1">D10/7</f>
-        <v>-1.8571428571428572</v>
+        <v>-2.8571428571428572</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.2">

</xml_diff>